<commit_message>
interim update for sim tracking
</commit_message>
<xml_diff>
--- a/sim_cfg/Possum_sim_tracking.xlsx
+++ b/sim_cfg/Possum_sim_tracking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Mean FD</t>
   </si>
@@ -67,6 +67,174 @@
   </si>
   <si>
     <t>fdM_target</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>job killed: walltime 194464 exceeded limit 194400</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=208Fetch_fdM95pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>job killed: walltime 331202 exceeded limit 331200</t>
+  </si>
+  <si>
+    <t>507 procs complete</t>
+  </si>
+  <si>
+    <t>job killed: cpuset memory_pressure 7505 reached/exceeded limit 1 (numa memused is 939397568 kb)</t>
+  </si>
+  <si>
+    <t>25 procs complete</t>
+  </si>
+  <si>
+    <t>ofile</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o307379</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o307378</t>
+  </si>
+  <si>
+    <t>9 procs complete</t>
+  </si>
+  <si>
+    <t>job killed: cpuset memory_pressure 121630 reached/exceeded limit 1 (numa memused is 938723452 kb)</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o306751</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=101Fetch_fdM25pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o306748</t>
+  </si>
+  <si>
+    <t>job killed: cpuset memory_pressure 20233 reached/exceeded limit 1 (numa memused is 935749624 kb)</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10604_fdM50pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>13 procs complete</t>
+  </si>
+  <si>
+    <t>job killed: walltime 194442 exceeded limit 194400</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=132Oddball_fdM90pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o306744</t>
+  </si>
+  <si>
+    <t>job killed: cpuset memory_pressure 49985 reached/exceeded limit 1 (numa memused is 939204128 kb)</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10818_fdM75pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>RECALCULATED SUSAN MOTION PARAMS BECAUSE MISSING REFERENCE ROW</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/210_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=210Oddball_fdM99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>killed manually because 511 completed, wasting CPU time</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o320038</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o306741; qsub_possum4d.bash.o320020</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o306681; qsub_possum4d.bash.o320018</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Oddball Movement/210_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>511 complete</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10678_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10678_fdM75pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>QUEUED</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/123_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>RUNNING</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=123Fetch_fdM50pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>/perlman_motfiles/Fetch Movement/223_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=223Fetch_fdM25pct_roiAvg_fulFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>pctile</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/120_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>fdCensPct</t>
+  </si>
+  <si>
+    <t>FD Percentage Censored &gt; 0.5mm (percentile)</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/119_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/113_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Oddball Movement/127_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10790_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10599_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=113Fetch_fdCenpct90pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=120Fetch_fdCenpct99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=119Fetch_fdCenpct95pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10599_fdCenpct25pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -76,7 +244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,13 +276,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,7 +319,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,25 +333,221 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -499,12 +888,12 @@
     <col min="1" max="1" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -521,38 +910,56 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>2.3674537</v>
+        <v>1.421557</v>
       </c>
       <c r="C4">
         <v>0.99</v>
       </c>
       <c r="D4" s="2">
-        <v>0.99436619999999998</v>
+        <v>0.99115039999999999</v>
       </c>
       <c r="E4" s="2">
-        <v>4.3661969999999996E-3</v>
+        <v>1.150442E-3</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -563,13 +970,25 @@
         <v>0.95</v>
       </c>
       <c r="D5" s="2">
-        <v>0.96338029999999997</v>
+        <v>0.95575220000000005</v>
       </c>
       <c r="E5" s="2">
-        <v>1.33802817E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>5.7522119999999996E-3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -580,64 +999,94 @@
         <v>0.9</v>
       </c>
       <c r="D6" s="2">
-        <v>0.92676060000000005</v>
+        <v>0.90707959999999999</v>
       </c>
       <c r="E6" s="2">
-        <v>2.6760563000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>7.0796460000000002E-3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B7">
-        <v>0.33310590000000001</v>
+        <v>0.33218399999999998</v>
       </c>
       <c r="C7">
         <v>0.75</v>
       </c>
       <c r="D7" s="2">
-        <v>0.74782610000000005</v>
+        <v>0.7477876</v>
       </c>
       <c r="E7" s="2">
-        <v>2.173913E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>2.2123889999999999E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B8">
-        <v>0.19950970000000001</v>
+        <v>0.1951436</v>
       </c>
       <c r="C8">
         <v>0.5</v>
       </c>
       <c r="D8" s="2">
-        <v>0.5</v>
+        <v>0.49557519999999999</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>4.4247790000000002E-3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B9">
-        <v>0.14555699999999999</v>
+        <v>0.14427789999999999</v>
       </c>
       <c r="C9">
         <v>0.25</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.25217390000000001</v>
+      <c r="D9" s="7">
+        <v>0.2477876</v>
       </c>
       <c r="E9" s="2">
-        <v>2.173913E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>2.2123889999999999E-3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -648,13 +1097,326 @@
         <v>0.1</v>
       </c>
       <c r="D10" s="2">
-        <v>0.109859</v>
+        <v>0.101769912</v>
       </c>
       <c r="E10" s="2">
-        <v>9.8499999999999994E-3</v>
+        <v>1.769912E-3</v>
       </c>
       <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
         <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.63333329999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.99</v>
+      </c>
+      <c r="D14">
+        <v>0.99115039999999999</v>
+      </c>
+      <c r="E14">
+        <v>1.150442E-3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>0.43333329999999998</v>
+      </c>
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="D15">
+        <v>0.95132740000000005</v>
+      </c>
+      <c r="E15">
+        <v>1.3274339999999999E-3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>0.3333333</v>
+      </c>
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+      <c r="D16">
+        <v>0.89823010000000003</v>
+      </c>
+      <c r="E16">
+        <v>1.769912E-3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
+      </c>
+      <c r="D17">
+        <v>0.7477876</v>
+      </c>
+      <c r="E17">
+        <v>2.2123889999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>0.49115039999999999</v>
+      </c>
+      <c r="E18">
+        <v>8.8495580000000004E-3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
+      <c r="D19">
+        <v>0.26106190000000001</v>
+      </c>
+      <c r="E19">
+        <v>1.1061949999999999E-2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>2.3674537</v>
+      </c>
+      <c r="C29">
+        <v>0.99</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.99436619999999998</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4.3661969999999996E-3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>0.33310590000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.75</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.74782610000000005</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.173913E-3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>0.19950970000000001</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>1.9668886000000001</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.99154929999999997</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1.5492959999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>0.14555699999999999</v>
+      </c>
+      <c r="C33">
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.25217390000000001</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2.173913E-3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Possum sim tracking update
</commit_message>
<xml_diff>
--- a/sim_cfg/Possum_sim_tracking.xlsx
+++ b/sim_cfg/Possum_sim_tracking.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>Mean FD</t>
   </si>
@@ -174,67 +174,145 @@
     <t>qsub -v SIMRUN=10678_fdM75pct_roiAvg_fullFreq qsub_possum4d.bash</t>
   </si>
   <si>
+    <t>perlman_motfiles/Fetch Movement/123_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=123Fetch_fdM50pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=223Fetch_fdM25pct_roiAvg_fulFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>pctile</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/120_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>fdCensPct</t>
+  </si>
+  <si>
+    <t>FD Percentage Censored &gt; 0.5mm (percentile)</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/119_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/113_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Oddball Movement/127_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10790_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10599_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=113Fetch_fdCenpct90pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=120Fetch_fdCenpct99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=119Fetch_fdCenpct95pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10599_fdCenpct25pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324938</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324921</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=127Oddball_fdCenpct75pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o325006</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324994</t>
+  </si>
+  <si>
+    <t>job killed: walltime 331270 exceeded limit 331200</t>
+  </si>
+  <si>
+    <t>502 complete</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324991</t>
+  </si>
+  <si>
+    <t>job killed: walltime 331281 exceeded limit 331200</t>
+  </si>
+  <si>
+    <t>THIS ONE MAY BE IMPOSSIBLE…. Only 52 procs completed, which means some ran all 92hours without completion</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o325004</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10790_fdCenpct50pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324984</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o324909</t>
+  </si>
+  <si>
+    <t>JOB DIED UNEXPECTEDLY</t>
+  </si>
+  <si>
+    <t>STALLED</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o325002, qsub_possum4d.bash.o330170</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10807_fdCenpct99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>507 complete</t>
+  </si>
+  <si>
+    <t>qsub_possum4d.bash.o330186</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Fetch Movement/223_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10807_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>rewRest_mot4d/10662_mt4d_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=224Oddball_fdM99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
     <t>QUEUED</t>
   </si>
   <si>
-    <t>perlman_motfiles/Fetch Movement/123_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>RUNNING</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=123Fetch_fdM50pct_roiAvg_fullFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>/perlman_motfiles/Fetch Movement/223_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=223Fetch_fdM25pct_roiAvg_fulFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>pctile</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>perlman_motfiles/Fetch Movement/120_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>fdCensPct</t>
-  </si>
-  <si>
-    <t>FD Percentage Censored &gt; 0.5mm (percentile)</t>
-  </si>
-  <si>
-    <t>perlman_motfiles/Fetch Movement/119_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>perlman_motfiles/Fetch Movement/113_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>perlman_motfiles/Oddball Movement/127_3DMC_FD.1D</t>
-  </si>
-  <si>
-    <t>rewRest_mot4d/10790_mt4d_FD.1D</t>
-  </si>
-  <si>
-    <t>rewRest_mot4d/10599_mt4d_FD.1D</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=113Fetch_fdCenpct90pct_roiAvg_fullFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=120Fetch_fdCenpct99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=119Fetch_fdCenpct95pct_roiAvg_fullFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>qsub -v SIMRUN=10599_fdCenpct25pct_roiAvg_fullFreq qsub_possum4d.bash</t>
-  </si>
-  <si>
-    <t>COMPLETE</t>
+    <t>perlman_motfiles/Oddball Movement/224_3DMC_FD.1D</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=10662_fdCenpct99pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>qsub -v SIMRUN=133Oddball_fdM95pct_roiAvg_fullFreq qsub_possum4d.bash</t>
+  </si>
+  <si>
+    <t>perlman_motfiles/Oddball Movement/133_3DMC_FD.1D</t>
   </si>
 </sst>
 </file>
@@ -284,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +387,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -319,7 +403,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -427,8 +511,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -440,8 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -495,6 +614,23 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -548,6 +684,23 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -888,12 +1041,12 @@
     <col min="1" max="1" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -922,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -930,7 +1083,7 @@
       <c r="E3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -946,7 +1099,7 @@
       <c r="E4" s="2">
         <v>1.150442E-3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="G4" t="s">
@@ -959,463 +1112,606 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.99</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.98670000000000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.2699999999999999E-3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.90278860000000005</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>0.95</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>0.95575220000000005</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>5.7522119999999996E-3</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>0.87762819999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.95</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.95132740000000005</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.3270000000000001E-3</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>0.6487946</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>0.9</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="2">
         <v>0.90707959999999999</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E8" s="2">
         <v>7.0796460000000002E-3</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>0.33218399999999998</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>0.75</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="2">
         <v>0.7477876</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.2123889999999999E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8">
-        <v>0.1951436</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.49557519999999999</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4.4247790000000002E-3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>0.14427789999999999</v>
-      </c>
-      <c r="C9">
-        <v>0.25</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.2477876</v>
       </c>
       <c r="E9" s="2">
         <v>2.2123889999999999E-3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>0.1951436</v>
+      </c>
+      <c r="C10">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.49557519999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.4247790000000002E-3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11">
+        <v>0.14427789999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.2477876</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.2123889999999999E-3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>8.701275E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.101769912</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.769912E-3</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>8.701275E-2</v>
-      </c>
-      <c r="C10">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.101769912</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.769912E-3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="B16" s="2">
         <v>0.63333329999999999</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>0.99</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>0.99115039999999999</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>1.150442E-3</v>
       </c>
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15">
-        <v>0.43333329999999998</v>
-      </c>
-      <c r="C15">
-        <v>0.95</v>
-      </c>
-      <c r="D15">
-        <v>0.95132740000000005</v>
-      </c>
-      <c r="E15">
-        <v>1.3274339999999999E-3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16">
-        <v>0.3333333</v>
-      </c>
-      <c r="C16">
-        <v>0.9</v>
-      </c>
-      <c r="D16">
-        <v>0.89823010000000003</v>
-      </c>
-      <c r="E16">
-        <v>1.769912E-3</v>
-      </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="B17">
-        <v>0.14000000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="C17">
-        <v>0.75</v>
+        <v>0.99</v>
       </c>
       <c r="D17">
-        <v>0.7477876</v>
+        <v>0.98672570000000004</v>
       </c>
       <c r="E17">
-        <v>2.2123889999999999E-3</v>
+        <v>3.2743360000000001E-3</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B18">
-        <v>3.5000000000000003E-2</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.99</v>
       </c>
       <c r="D18">
-        <v>0.49115039999999999</v>
+        <v>0.99557519999999999</v>
       </c>
       <c r="E18">
-        <v>8.8495580000000004E-3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>51</v>
+        <v>5.5750000000000001E-3</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>0.43333329999999998</v>
+      </c>
+      <c r="C19">
+        <v>0.95</v>
+      </c>
+      <c r="D19">
+        <v>0.95132740000000005</v>
+      </c>
+      <c r="E19">
+        <v>1.3274339999999999E-3</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" t="s">
         <v>66</v>
       </c>
-      <c r="B19">
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20">
+        <v>0.3333333</v>
+      </c>
+      <c r="C20">
+        <v>0.9</v>
+      </c>
+      <c r="D20">
+        <v>0.89823010000000003</v>
+      </c>
+      <c r="E20">
+        <v>1.769912E-3</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0.75</v>
+      </c>
+      <c r="D21">
+        <v>0.7477876</v>
+      </c>
+      <c r="E21">
+        <v>2.2123889999999999E-3</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>0.49115039999999999</v>
+      </c>
+      <c r="E22">
+        <v>8.8495580000000004E-3</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C19">
+      <c r="C23">
         <v>0.25</v>
       </c>
-      <c r="D19">
+      <c r="D23">
         <v>0.26106190000000001</v>
       </c>
-      <c r="E19">
+      <c r="E23">
         <v>1.1061949999999999E-2</v>
       </c>
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+      <c r="F23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>2.3674537</v>
-      </c>
-      <c r="C29">
-        <v>0.99</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.99436619999999998</v>
-      </c>
-      <c r="E29" s="2">
-        <v>4.3661969999999996E-3</v>
-      </c>
-      <c r="F29" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30">
-        <v>0.33310590000000001</v>
-      </c>
-      <c r="C30">
-        <v>0.75</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.74782610000000005</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2.173913E-3</v>
-      </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" t="s">
-        <v>39</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <v>0.19950970000000001</v>
-      </c>
-      <c r="C31">
-        <v>0.5</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32">
-        <v>1.9668886000000001</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0.99</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.99154929999999997</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1.5492959999999999E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>2.3674537</v>
+      </c>
+      <c r="C33">
+        <v>0.99</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.99436619999999998</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4.3661969999999996E-3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>0.33310590000000001</v>
+      </c>
+      <c r="C34">
+        <v>0.75</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.74782610000000005</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.173913E-3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>0.19950970000000001</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>1.9668886000000001</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.99154929999999997</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.5492959999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B33">
+      <c r="B37">
         <v>0.14555699999999999</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <v>0.25</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D37" s="2">
         <v>0.25217390000000001</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E37" s="2">
         <v>2.173913E-3</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F37" t="s">
         <v>27</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G37" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I37" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>